<commit_message>
update the wind extraction
</commit_message>
<xml_diff>
--- a/protection_zones_without_AB1.xlsx
+++ b/protection_zones_without_AB1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masterthesis\IEET\pycharmtest\backup_code_masterthesis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04382219-1DFF-4D75-927C-EB0FAA390604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -127,12 +133,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -140,8 +146,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -191,13 +204,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +256,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -269,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -303,9 +325,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,14 +501,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -528,7 +555,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -548,7 +575,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -568,7 +595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -588,7 +615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -608,7 +635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -628,7 +655,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -648,7 +675,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -668,7 +695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -688,7 +715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -708,7 +735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -728,7 +755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -748,7 +775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -771,7 +798,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -794,7 +821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -814,7 +841,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -835,6 +862,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>